<commit_message>
1st attempt at PI control
</commit_message>
<xml_diff>
--- a/duty_vs_speed.xlsx
+++ b/duty_vs_speed.xlsx
@@ -12,16 +12,20 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr autoRecover="0" repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>DUTY</t>
   </si>
   <si>
     <t>SPEED</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -306,11 +310,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="38886784"/>
-        <c:axId val="38921344"/>
+        <c:axId val="85661568"/>
+        <c:axId val="85676032"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="38886784"/>
+        <c:axId val="85661568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -339,7 +343,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="38921344"/>
+        <c:crossAx val="85676032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -347,7 +351,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="38921344"/>
+        <c:axId val="85676032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -358,7 +362,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="38886784"/>
+        <c:crossAx val="85661568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -401,8 +405,8 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -418,9 +422,16 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:trendline>
             <c:trendlineType val="linear"/>
             <c:dispRSqr val="0"/>
@@ -428,14 +439,14 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.17608945756780403"/>
+                  <c:x val="-7.2108267716535432E-2"/>
                   <c:y val="-3.5906969962088071E-4"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$A$7:$A$22</c:f>
               <c:numCache>
@@ -491,8 +502,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>Sheet1!$B$7:$B$22</c:f>
               <c:numCache>
@@ -548,7 +559,7 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
@@ -559,13 +570,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="44388352"/>
-        <c:axId val="44389888"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="44388352"/>
+        <c:axId val="85705472"/>
+        <c:axId val="85707008"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="85705472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -575,15 +584,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44389888"/>
+        <c:crossAx val="85707008"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
-        <c:axId val="44389888"/>
+        <c:axId val="85707008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -594,13 +600,17 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44388352"/>
+        <c:crossAx val="85705472"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:legendEntry>
+        <c:idx val="1"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
       <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
@@ -608,6 +618,35 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="accent5"/>
+      </a:solidFill>
+      <a:prstDash val="solid"/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:solidFill>
+            <a:schemeClr val="dk1"/>
+          </a:solidFill>
+          <a:latin typeface="+mn-lt"/>
+          <a:ea typeface="+mn-ea"/>
+          <a:cs typeface="+mn-cs"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -968,10 +1007,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P27" sqref="P27"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1108,7 +1147,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>75</v>
       </c>
@@ -1116,7 +1155,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>80</v>
       </c>
@@ -1124,7 +1163,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>85</v>
       </c>
@@ -1132,7 +1171,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>90</v>
       </c>
@@ -1140,7 +1179,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>95</v>
       </c>
@@ -1148,12 +1187,17 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>100</v>
       </c>
       <c r="B22" s="2">
         <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F27" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>